<commit_message>
Deploying to gh-pages from @ Atmelfan/pcb-adr1399-vref@42d1b3c6a442e3b5243eb42099689c064005cf90 🚀
</commit_message>
<xml_diff>
--- a/docs/bom/pcb-adr1399-vref-kicost.xlsx
+++ b/docs/bom/pcb-adr1399-vref-kicost.xlsx
@@ -1610,7 +1610,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Thu Feb  3 20:37:07 2022</t>
+    <t>Thu Feb  3 21:45:12 2022</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1625,7 +1625,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-02-03 20:37:09</t>
+    <t>2022-02-03 21:45:13</t>
   </si>
   <si>
     <t>Arrow</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Atmelfan/pcb-adr1399-vref@9785d729a6f2eb738e8dea6960c3aa0cc603fe6b 🚀
</commit_message>
<xml_diff>
--- a/docs/bom/pcb-adr1399-vref-kicost.xlsx
+++ b/docs/bom/pcb-adr1399-vref-kicost.xlsx
@@ -1610,7 +1610,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Thu Feb  3 21:59:40 2022</t>
+    <t>Thu Feb  3 22:06:54 2022</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1625,7 +1625,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-02-03 21:59:42</t>
+    <t>2022-02-03 22:06:55</t>
   </si>
   <si>
     <t>Arrow</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Atmelfan/pcb-adr1399-vref@a7292277256407f949378d21e8d5ccdddb0bd8f4 🚀
</commit_message>
<xml_diff>
--- a/docs/bom/pcb-adr1399-vref-kicost.xlsx
+++ b/docs/bom/pcb-adr1399-vref-kicost.xlsx
@@ -1610,7 +1610,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Thu Feb  3 22:06:54 2022</t>
+    <t>Fri Feb  4 23:08:02 2022</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1625,7 +1625,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-02-03 22:06:55</t>
+    <t>2022-02-04 23:08:03</t>
   </si>
   <si>
     <t>Arrow</t>
@@ -3485,7 +3485,7 @@
         <v>52</v>
       </c>
       <c r="C24">
-        <v>1.201807518507836</v>
+        <v>1.182130909176882</v>
       </c>
       <c r="F24" s="22" t="s">
         <v>50</v>
@@ -3530,7 +3530,7 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>0.886053517632465</v>
+        <v>0.8722958827634333</v>
       </c>
       <c r="I25">
         <f t="array" ref="I25">IFERROR(CONCATENATE(INDEX(L7:L21,SMALL(IF(ISNUMBER(I7:I21),IF(I7:I21&gt;0,IF(L7:L21&lt;&gt;"",ROW(I7:I21)-MIN(ROW(I7:I21))+1))),ROW()-ROW(A$24)+1)),",",TEXT(INDEX(I7:I21,SMALL(IF(ISNUMBER(I7:I21),IF(I7:I21&gt;0,IF(L7:L21&lt;&gt;"",ROW(I7:I21)-MIN(ROW(I7:I21))+1))),ROW()-ROW(A$24)+1)),"##0"),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A21,SMALL(IF(ISNUMBER(I7:I21),IF(I7:I21&gt;0,IF(L7:L21&lt;&gt;"",ROW(I7:I21)-MIN(ROW(I7:I21))+1))),ROW()-ROW(A$24)+1)),",",";")),"")</f>

</xml_diff>